<commit_message>
Regenerat SML IG outputs
Further updates from peer review
CIFMM-2576
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/substance-dh-base-1.xlsx
+++ b/output/SharedMedicinesList/substance-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$30</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="199">
   <si>
     <t>Path</t>
   </si>
@@ -428,13 +428,10 @@
     <t>This could be a reference to an externally defined code.  It could also be a locally assigned code (e.g. a formulary),  optionally with translations to the standard drug codes.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Substance codes</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/substance-code</t>
+    <t>preferred</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/substance-1</t>
   </si>
   <si>
     <t>fhir:Substance.code rdfs:subPropertyOf rim:Entity.code</t>
@@ -614,10 +611,33 @@
     <t>Another substance that is a component of this substance.</t>
   </si>
   <si>
+    <t>example</t>
+  </si>
+  <si>
     <t>Substance Ingredient codes</t>
   </si>
   <si>
+    <t>http://hl7.org/fhir/ValueSet/substance-code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
     <t>.player</t>
+  </si>
+  <si>
+    <t>substanceCodeableConcept</t>
+  </si>
+  <si>
+    <t>substanceReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/StructureDefinition/au-substance)
+</t>
   </si>
 </sst>
 </file>
@@ -766,7 +786,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:AL30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -776,7 +796,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="36.8203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="25.83984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -799,7 +819,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="45.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="44.40234375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="56.859375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
@@ -2283,11 +2303,9 @@
       <c r="W14" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="X14" t="s" s="2">
+      <c r="X14" s="2"/>
+      <c r="Y14" t="s" s="2">
         <v>133</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>134</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>39</v>
@@ -2323,15 +2341,15 @@
         <v>126</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AL14" t="s" s="2">
         <v>135</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>136</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2354,13 +2372,13 @@
         <v>50</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="K15" t="s" s="2">
         <v>138</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="L15" t="s" s="2">
         <v>139</v>
-      </c>
-      <c r="L15" t="s" s="2">
-        <v>140</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2411,7 +2429,7 @@
         <v>39</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -2426,7 +2444,7 @@
         <v>39</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>39</v>
@@ -2437,7 +2455,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2460,13 +2478,13 @@
         <v>50</v>
       </c>
       <c r="J16" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="K16" t="s" s="2">
         <v>143</v>
       </c>
-      <c r="K16" t="s" s="2">
+      <c r="L16" t="s" s="2">
         <v>144</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>145</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2474,7 +2492,7 @@
         <v>39</v>
       </c>
       <c r="P16" t="s" s="2">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Q16" t="s" s="2">
         <v>39</v>
@@ -2519,7 +2537,7 @@
         <v>39</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
@@ -2531,10 +2549,10 @@
         <v>39</v>
       </c>
       <c r="AI16" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AJ16" t="s" s="2">
         <v>147</v>
-      </c>
-      <c r="AJ16" t="s" s="2">
-        <v>148</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>39</v>
@@ -2545,7 +2563,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2568,13 +2586,13 @@
         <v>39</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K17" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2625,7 +2643,7 @@
         <v>39</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
@@ -2640,7 +2658,7 @@
         <v>39</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>39</v>
@@ -2651,7 +2669,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2680,7 +2698,7 @@
         <v>96</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M18" t="s" s="2">
         <v>98</v>
@@ -2733,7 +2751,7 @@
         <v>39</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
@@ -2748,7 +2766,7 @@
         <v>39</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>39</v>
@@ -2759,11 +2777,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -2788,7 +2806,7 @@
         <v>101</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>98</v>
@@ -2841,7 +2859,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -2867,7 +2885,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2893,10 +2911,10 @@
         <v>105</v>
       </c>
       <c r="K20" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>162</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>163</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2947,7 +2965,7 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -2973,7 +2991,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2996,13 +3014,13 @@
         <v>50</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="K21" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="L21" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>167</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3053,7 +3071,7 @@
         <v>39</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3068,7 +3086,7 @@
         <v>39</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>39</v>
@@ -3079,7 +3097,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3102,13 +3120,13 @@
         <v>50</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="K22" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="L22" t="s" s="2">
         <v>171</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>172</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3159,7 +3177,7 @@
         <v>39</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3174,7 +3192,7 @@
         <v>39</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>39</v>
@@ -3185,7 +3203,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3208,13 +3226,13 @@
         <v>50</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>174</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>175</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>176</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3265,7 +3283,7 @@
         <v>39</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3277,10 +3295,10 @@
         <v>39</v>
       </c>
       <c r="AI23" t="s" s="2">
+        <v>176</v>
+      </c>
+      <c r="AJ23" t="s" s="2">
         <v>177</v>
-      </c>
-      <c r="AJ23" t="s" s="2">
-        <v>178</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>39</v>
@@ -3291,7 +3309,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3314,13 +3332,13 @@
         <v>39</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>150</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>151</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3371,7 +3389,7 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3386,7 +3404,7 @@
         <v>39</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>39</v>
@@ -3397,7 +3415,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3426,7 +3444,7 @@
         <v>96</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M25" t="s" s="2">
         <v>98</v>
@@ -3479,7 +3497,7 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -3494,7 +3512,7 @@
         <v>39</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>39</v>
@@ -3505,11 +3523,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -3534,7 +3552,7 @@
         <v>101</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>98</v>
@@ -3587,7 +3605,7 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -3613,7 +3631,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3636,13 +3654,13 @@
         <v>50</v>
       </c>
       <c r="J27" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="K27" t="s" s="2">
         <v>183</v>
       </c>
-      <c r="K27" t="s" s="2">
+      <c r="L27" t="s" s="2">
         <v>184</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>185</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -3693,7 +3711,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -3708,18 +3726,18 @@
         <v>39</v>
       </c>
       <c r="AJ27" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="AK27" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" hidden="true">
+      <c r="A28" t="s" s="2">
         <v>186</v>
-      </c>
-      <c r="AK27" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="2">
-        <v>187</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3742,13 +3760,13 @@
         <v>50</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="K28" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="K28" t="s" s="2">
+      <c r="L28" t="s" s="2">
         <v>189</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>190</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -3775,31 +3793,29 @@
         <v>39</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>132</v>
+        <v>190</v>
       </c>
       <c r="X28" t="s" s="2">
         <v>191</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>39</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="AB28" s="2"/>
       <c r="AC28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>39</v>
+        <v>194</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>49</v>
@@ -3814,17 +3830,231 @@
         <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL28" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" hidden="true">
+      <c r="A29" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F29" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I29" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="J29" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W29" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="X29" s="2"/>
+      <c r="Y29" t="s" s="2">
+        <v>133</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" hidden="true">
+      <c r="A30" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="H30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="I30" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="J30" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="K30" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE30" t="s" s="2">
+        <v>186</v>
+      </c>
+      <c r="AF30" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
+        <v>195</v>
+      </c>
+      <c r="AK30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AL30" t="s" s="2">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL28">
+  <autoFilter ref="A1:AL30">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3834,7 +4064,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI27">
+  <conditionalFormatting sqref="A2:AI29">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Output following updated WIP CDA IGs tot he STU3 FHIR IGs
Generated output of all STU3 FHIR IGs following updating of WIP CDA IG's.  CIFMM-2839.
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/substance-dh-base-1.xlsx
+++ b/output/SharedMedicinesList/substance-dh-base-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AL$28</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="193">
   <si>
     <t>Path</t>
   </si>
@@ -428,10 +428,13 @@
     <t>This could be a reference to an externally defined code.  It could also be a locally assigned code (e.g. a formulary),  optionally with translations to the standard drug codes.</t>
   </si>
   <si>
-    <t>preferred</t>
-  </si>
-  <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/substance-1</t>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Substance codes</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/substance-code</t>
   </si>
   <si>
     <t>fhir:Substance.code rdfs:subPropertyOf rim:Entity.code</t>
@@ -611,33 +614,10 @@
     <t>Another substance that is a component of this substance.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
     <t>Substance Ingredient codes</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/substance-code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
     <t>.player</t>
-  </si>
-  <si>
-    <t>substanceCodeableConcept</t>
-  </si>
-  <si>
-    <t>substanceReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(http://hl7.org.au/fhir/StructureDefinition/au-substance)
-</t>
   </si>
 </sst>
 </file>
@@ -786,7 +766,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL30"/>
+  <dimension ref="A1:AL28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -796,7 +776,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="36.8203125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="25.83984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -819,7 +799,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="45.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="56.859375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="44.40234375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="17.8203125" customWidth="true" bestFit="true"/>
@@ -2303,9 +2283,11 @@
       <c r="W14" t="s" s="2">
         <v>132</v>
       </c>
-      <c r="X14" s="2"/>
+      <c r="X14" t="s" s="2">
+        <v>133</v>
+      </c>
       <c r="Y14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>39</v>
@@ -2341,15 +2323,15 @@
         <v>126</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2372,13 +2354,13 @@
         <v>50</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2429,7 +2411,7 @@
         <v>39</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -2444,7 +2426,7 @@
         <v>39</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>39</v>
@@ -2455,7 +2437,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2478,13 +2460,13 @@
         <v>50</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2492,7 +2474,7 @@
         <v>39</v>
       </c>
       <c r="P16" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Q16" t="s" s="2">
         <v>39</v>
@@ -2537,7 +2519,7 @@
         <v>39</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>40</v>
@@ -2549,10 +2531,10 @@
         <v>39</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>39</v>
@@ -2563,7 +2545,7 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2586,13 +2568,13 @@
         <v>39</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2643,7 +2625,7 @@
         <v>39</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>40</v>
@@ -2658,7 +2640,7 @@
         <v>39</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>39</v>
@@ -2669,7 +2651,7 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2698,7 +2680,7 @@
         <v>96</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M18" t="s" s="2">
         <v>98</v>
@@ -2751,7 +2733,7 @@
         <v>39</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>40</v>
@@ -2766,7 +2748,7 @@
         <v>39</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>39</v>
@@ -2777,11 +2759,11 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
@@ -2806,7 +2788,7 @@
         <v>101</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M19" t="s" s="2">
         <v>98</v>
@@ -2859,7 +2841,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>40</v>
@@ -2885,7 +2867,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2911,10 +2893,10 @@
         <v>105</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2965,7 +2947,7 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -2991,7 +2973,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3014,13 +2996,13 @@
         <v>50</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -3071,7 +3053,7 @@
         <v>39</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>
@@ -3086,7 +3068,7 @@
         <v>39</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>39</v>
@@ -3097,7 +3079,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3120,13 +3102,13 @@
         <v>50</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3177,7 +3159,7 @@
         <v>39</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>40</v>
@@ -3192,7 +3174,7 @@
         <v>39</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>39</v>
@@ -3203,7 +3185,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3226,13 +3208,13 @@
         <v>50</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3283,7 +3265,7 @@
         <v>39</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>40</v>
@@ -3295,10 +3277,10 @@
         <v>39</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>39</v>
@@ -3309,7 +3291,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3332,13 +3314,13 @@
         <v>39</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3389,7 +3371,7 @@
         <v>39</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>40</v>
@@ -3404,7 +3386,7 @@
         <v>39</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>39</v>
@@ -3415,7 +3397,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3444,7 +3426,7 @@
         <v>96</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="M25" t="s" s="2">
         <v>98</v>
@@ -3497,7 +3479,7 @@
         <v>39</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>40</v>
@@ -3512,7 +3494,7 @@
         <v>39</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>39</v>
@@ -3523,11 +3505,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -3552,7 +3534,7 @@
         <v>101</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>98</v>
@@ -3605,7 +3587,7 @@
         <v>39</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>40</v>
@@ -3631,7 +3613,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3654,13 +3636,13 @@
         <v>50</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -3711,7 +3693,7 @@
         <v>39</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>40</v>
@@ -3726,7 +3708,7 @@
         <v>39</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AK27" t="s" s="2">
         <v>39</v>
@@ -3735,9 +3717,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" hidden="true">
+    <row r="28">
       <c r="A28" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3760,13 +3742,13 @@
         <v>50</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -3793,29 +3775,31 @@
         <v>39</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="X28" t="s" s="2">
         <v>191</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>192</v>
+        <v>134</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AA28" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="AB28" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="AB28" t="s" s="2">
+        <v>39</v>
+      </c>
       <c r="AC28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD28" t="s" s="2">
-        <v>194</v>
+        <v>39</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>49</v>
@@ -3830,231 +3814,17 @@
         <v>39</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" hidden="true">
-      <c r="A29" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="B29" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F29" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I29" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J29" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="K29" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P29" s="2"/>
-      <c r="Q29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W29" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="X29" s="2"/>
-      <c r="Y29" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="Z29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" hidden="true">
-      <c r="A30" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="C30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="F30" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="G30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="H30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="I30" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="J30" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="K30" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="P30" s="2"/>
-      <c r="Q30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="R30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="S30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="T30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="U30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="V30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="W30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="X30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Z30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ30" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AL30" t="s" s="2">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL30">
+  <autoFilter ref="A1:AL28">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -4064,7 +3834,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI29">
+  <conditionalFormatting sqref="A2:AI27">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>